<commit_message>
E-statement and Admin request accept done
</commit_message>
<xml_diff>
--- a/e-statement.xlsx
+++ b/e-statement.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Transaction ID</t>
   </si>
@@ -43,7 +43,7 @@
     <t>Transaction Charge</t>
   </si>
   <si>
-    <t>1648628301350</t>
+    <t>2022-06-14 16:13:20</t>
   </si>
   <si>
     <t>UNOL0000001</t>
@@ -58,19 +58,10 @@
     <t>IMPS</t>
   </si>
   <si>
-    <t>300</t>
+    <t>100</t>
   </si>
   <si>
     <t>Debit</t>
-  </si>
-  <si>
-    <t>1648630527061</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>1648885424980</t>
   </si>
 </sst>
 </file>
@@ -447,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="10" width="30" customWidth="1"/>
@@ -487,7 +478,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -514,70 +505,6 @@
         <v>16</v>
       </c>
       <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4">
         <v>0</v>
       </c>
     </row>

</xml_diff>